<commit_message>
Tavish, Testing, Results, Filters
</commit_message>
<xml_diff>
--- a/02-FIlters/Filter Materials 202005.xlsx
+++ b/02-FIlters/Filter Materials 202005.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wckng/Reusable-N95-Project/02-FIlters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4EBD92-9C20-0D4B-AB5A-8B5AE8B15F87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F08457-0DC0-F84A-A6CF-07F46BF3B529}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{A67B9D13-B8C8-CB44-8E2C-30A23EDF9F74}"/>
+    <workbookView xWindow="-10480" yWindow="-25020" windowWidth="31200" windowHeight="19220" xr2:uid="{A67B9D13-B8C8-CB44-8E2C-30A23EDF9F74}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
+    <sheet name="FF Testing" sheetId="2" r:id="rId2"/>
+    <sheet name="CFD Testing" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -85,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="92">
   <si>
     <t>Material Mastersheet</t>
   </si>
@@ -150,9 +152,6 @@
     <t>www.medi-select.ca</t>
   </si>
   <si>
-    <t>MERV-8</t>
-  </si>
-  <si>
     <t>Quang</t>
   </si>
   <si>
@@ -286,13 +285,91 @@
   </si>
   <si>
     <t>Will Ng</t>
+  </si>
+  <si>
+    <t>MERV-8 Enduropleat</t>
+  </si>
+  <si>
+    <t>MERV-8 Aerostar</t>
+  </si>
+  <si>
+    <t>Ridg10</t>
+  </si>
+  <si>
+    <t>wired</t>
+  </si>
+  <si>
+    <t>Containe Filter</t>
+  </si>
+  <si>
+    <t>red-tab</t>
+  </si>
+  <si>
+    <t>black-tab</t>
+  </si>
+  <si>
+    <t>unprocessed</t>
+  </si>
+  <si>
+    <t>processed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtration Factor Testing.  60mL (BD Luer Lock) syringe, occluded on one end.  Filter material tightly taped over open end with packing tape.  Sampling line inserted through hole in sidewall of syringe </t>
+  </si>
+  <si>
+    <t>Machine - AccuFit 9000 (Levitt Safety)</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Location:</t>
+  </si>
+  <si>
+    <t>Toronto General Hospital, Department of Anesthesia</t>
+  </si>
+  <si>
+    <t>Testers:</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>WN</t>
+  </si>
+  <si>
+    <t>Filtration Factor (Outside particulate concentration : Inside particulate concentration, averaged by integral/time)</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Overall Filtration Factor</t>
+  </si>
+  <si>
+    <t>Average Filtration Factor</t>
+  </si>
+  <si>
+    <t>Note 1 - first 3 measurements used as equilibration time, and not included in average</t>
+  </si>
+  <si>
+    <t>Note 2</t>
+  </si>
+  <si>
+    <t>Overall Filtration Factor is given by a formula, where n= no. of runs, here n=7:</t>
+  </si>
+  <si>
+    <t>Overall FF = 1/(1/ff1 + 1/ff2 + 1/ff3 + 1/ff4 + 1/ff5 + 1/ff6 +1/ff7)</t>
+  </si>
+  <si>
+    <t>IGNORE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -329,16 +406,36 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -346,16 +443,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -671,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF48A646-0DC7-9043-94D4-6A4F0712B920}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,7 +820,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3">
         <v>43955</v>
@@ -705,10 +828,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -786,219 +909,213 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>21</v>
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D13" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
         <v>25</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13" t="s">
         <v>26</v>
       </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
         <v>27</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
-      </c>
-      <c r="H11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>32</v>
-      </c>
-      <c r="L11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12">
-        <v>4</v>
-      </c>
-      <c r="H12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="C19" t="s">
         <v>42</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D19" t="s">
         <v>43</v>
-      </c>
-      <c r="D16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
       </c>
       <c r="E19" t="s">
         <v>16</v>
@@ -1008,23 +1125,14 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -1032,36 +1140,47 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
       </c>
-      <c r="F21" t="s">
-        <v>26</v>
-      </c>
       <c r="J21">
         <v>0</v>
       </c>
-      <c r="K21" t="s">
-        <v>54</v>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" t="s">
         <v>51</v>
-      </c>
-      <c r="F23" t="s">
-        <v>58</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1069,33 +1188,73 @@
       <c r="J23">
         <v>0</v>
       </c>
-      <c r="K23" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1105,4 +1264,420 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE99BBC-E01C-7443-B17C-8673EE96DE37}">
+  <dimension ref="A1:U23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="9">
+        <v>43956</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="S4" s="3"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>2</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+    </row>
+    <row r="16" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+    </row>
+    <row r="17" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="11" t="e">
+        <f>AVERAGE(B11:B14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C17" s="11" t="e">
+        <f t="shared" ref="C17:M17" si="0">AVERAGE(C11:C14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D17" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E17" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F17" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K17" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L17" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N17" s="10"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:M6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA75BC21-C97C-974B-9DC9-BEB5473524A4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>